<commit_message>
Update DR# 719 BDO UNIBANK GEMALTO(Virtual Cards MC - BDO Virtual Cards VISA)_03-04_2022.xlsx
</commit_message>
<xml_diff>
--- a/DR# 719 BDO UNIBANK GEMALTO(Virtual Cards MC - BDO Virtual Cards VISA)_03-04_2022.xlsx
+++ b/DR# 719 BDO UNIBANK GEMALTO(Virtual Cards MC - BDO Virtual Cards VISA)_03-04_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime Ponio IV\Documents\GitHub\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE3076D5-559E-4256-987E-9018BCCCA469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A5DFF5-B881-4B5A-9ADC-231EA7F58C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1597,8 +1597,8 @@
     <mergeCell ref="A11:M11"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>